<commit_message>
income affordability file with 60%ami information added
</commit_message>
<xml_diff>
--- a/Data/incomeAffordability.xlsx
+++ b/Data/incomeAffordability.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taohe/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taohe/Documents/GitHub/SLC-Housing-Dashboard/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A6877D48-2AD5-3D47-B1EB-A70D6D76E5A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15560"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Year</t>
   </si>
@@ -35,9 +36,6 @@
     <t>80AMI</t>
   </si>
   <si>
-    <t>Affordability</t>
-  </si>
-  <si>
     <t>MedianSale</t>
   </si>
   <si>
@@ -48,12 +46,18 @@
   </si>
   <si>
     <t>3BRAveRent</t>
+  </si>
+  <si>
+    <t>80Affordability</t>
+  </si>
+  <si>
+    <t>60Affordability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -398,16 +402,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,22 +422,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -455,10 +462,13 @@
         <v>45240</v>
       </c>
       <c r="G2">
+        <v>190400</v>
+      </c>
+      <c r="H2">
         <f>F2*0.3/12</f>
         <v>1131</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1910</v>
       </c>
     </row>

</xml_diff>